<commit_message>
carga de planillas 1º
</commit_message>
<xml_diff>
--- a/proyectoCalificador-root/devPlanillas/planillaBase.xlsx
+++ b/proyectoCalificador-root/devPlanillas/planillaBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitProjects\proyectoCalificador\proyectoCalificador-root\devPlanillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEC45CD-4D66-4FF9-B810-D8E156F664FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693A20C5-7CBF-4246-89E1-9036EAAF900A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18510" yWindow="480" windowWidth="5505" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="156">
   <si>
     <t>DNI</t>
   </si>
@@ -331,6 +331,180 @@
   </si>
   <si>
     <t xml:space="preserve"> 18/12/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FACUNDO NATANAEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24/02/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CINTIA YUSIELI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13/10/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LEONEL GONZALO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25/04/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SAMUEL ALEJANDRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23/02/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EMANUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 08/02/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EZEQUIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LUDMILA ANDREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03/10/2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARTIN LEONEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/01/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LAUTARO MIGUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ELIEZER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 30/08/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LUCAS NAHUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 30/06/2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ELISAMA ESTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 05/09/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DENIS NAHUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GUSTAVO REUEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/08/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ERIKA ROCIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/06/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LAUTARO EZEQUIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 30/07/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NAHIARA AGUSTINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AXEL GABRIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/05/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ESMERALDA ELENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21/11/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DAMARIS BELEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19/03/2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ARIEL ADRIAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/04/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JOSIAS GABRIEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27/07/2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ALVEZ FIGUEIRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AMARO DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BATISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BIANCHI SALAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CAMPOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DA CRUZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DA SILVA RODRIGUEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DA SILVEIRA QUADRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DE OLIVERA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DUTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FICHTNER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GARCIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GOMEZ CABAÑA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LEMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PEREIRA ROWAHYAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> QUIROZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RIVAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SOSA</t>
   </si>
 </sst>
 </file>
@@ -371,12 +545,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -662,478 +846,392 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D33"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>50660080</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+      <c r="A2" s="4">
+        <v>50819016</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>50816657</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
+      <c r="A3" s="4">
+        <v>50571983</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>51076611</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
+      <c r="A4" s="4">
+        <v>51076650</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>50940302</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
+      <c r="A5" s="4">
+        <v>50922334</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>51220176</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
+      <c r="A6" s="4">
+        <v>50164332</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>50429709</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
+      <c r="A7" s="4">
+        <v>50164331</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>51212019</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
+      <c r="A8" s="4">
+        <v>49691660</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>50429618</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
+      <c r="A9" s="4">
+        <v>50730897</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>50344338</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="4">
+        <v>50660029</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>50429781</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>49691599</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>50660003</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>50660015</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>50941409</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>51076873</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>51076878</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>51076664</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>50940335</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>45</v>
+      <c r="A15" s="4">
+        <v>49992546</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>50521874</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>48</v>
+      <c r="A16" s="4">
+        <v>51115874</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>50940316</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>51</v>
+      <c r="A17" s="4">
+        <v>50429724</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>50731121</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>54</v>
+      <c r="A18" s="4">
+        <v>50571985</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>50660832</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>57</v>
+      <c r="A19" s="4">
+        <v>50344309</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>50429749</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>60</v>
+      <c r="A20" s="4">
+        <v>50660191</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>50345675</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>63</v>
+      <c r="A21" s="4">
+        <v>50819071</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>50730876</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>66</v>
+      <c r="A22" s="4">
+        <v>50164094</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>50660852</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>69</v>
+      <c r="A23" s="4">
+        <v>50344396</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>51076623</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>51076801</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>50571991</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>51076692</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>50344375</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>50660010</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>50867839</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>50359661</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>50967678</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="A32" s="6"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>50660881</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="A33" s="6"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1145,8 +1243,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>